<commit_message>
Remove emissions from H2 train
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-rail-freight.xlsx
+++ b/premise/data/additional_inventories/lci-rail-freight.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6773C0A-3032-5644-9A31-EA25FAA30787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EFDAEB-930B-404E-800F-42C66BFE2A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="1860" windowWidth="22100" windowHeight="17540" xr2:uid="{3988C069-CC65-40BA-9751-20608AAA2DA4}"/>
+    <workbookView xWindow="8140" yWindow="1860" windowWidth="22100" windowHeight="17540" xr2:uid="{3988C069-CC65-40BA-9751-20608AAA2DA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="280">
   <si>
     <t>Activity</t>
   </si>
@@ -1041,11 +1041,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A08E695-FC79-4DF0-ACCB-3B3F78317B74}">
   <dimension ref="A1:H943"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1880,7 +1879,7 @@
       <c r="A41" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3799,6 +3798,9 @@
       </c>
       <c r="D149" t="s">
         <v>278</v>
+      </c>
+      <c r="E149" t="s">
+        <v>240</v>
       </c>
       <c r="F149" t="s">
         <v>73</v>

</xml_diff>